<commit_message>
updating ISA format macros in header files; small updates to the opcodes table; adding a few additional options to main source file
</commit_message>
<xml_diff>
--- a/sim/goblin-core_opcodes.xlsx
+++ b/sim/goblin-core_opcodes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23580" windowHeight="13360" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23580" windowHeight="13360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="666">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2125,9 +2125,6 @@
   </si>
   <si>
     <t xml:space="preserve">software scratchpad? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">network addressing? </t>
   </si>
   <si>
     <t>VL</t>
@@ -2626,8 +2623,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2872,6 +2871,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2881,10 +2884,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2894,11 +2896,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2989,6 +2988,7 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3079,6 +3079,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3410,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3434,12 +3435,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -3662,17 +3663,17 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>651</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>652</v>
       </c>
       <c r="C11" s="22">
         <v>16</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>650</v>
+      <c r="D11" s="29" t="s">
+        <v>649</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -4156,17 +4157,14 @@
       </c>
     </row>
     <row r="45" spans="4:12">
-      <c r="D45" t="s">
-        <v>605</v>
-      </c>
       <c r="F45" s="6" t="s">
         <v>70</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>156</v>
@@ -4177,52 +4175,52 @@
         <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="36" t="s">
-        <v>661</v>
+      <c r="D47" s="33" t="s">
+        <v>660</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I47" s="19" t="s">
         <v>156</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="36"/>
+      <c r="D48" s="33"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>627</v>
-      </c>
       <c r="I48" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="36"/>
+      <c r="D49" s="33"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
@@ -4237,37 +4235,37 @@
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="36"/>
+      <c r="D50" s="33"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="36"/>
+      <c r="D51" s="33"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G51" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="H51" s="7" t="s">
-        <v>616</v>
-      </c>
       <c r="I51" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="36"/>
+      <c r="D52" s="33"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4282,7 +4280,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="36"/>
+      <c r="D53" s="33"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4297,7 +4295,7 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="36"/>
+      <c r="D54" s="33"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
@@ -4470,10 +4468,10 @@
         <v>91</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>321</v>
@@ -4512,76 +4510,76 @@
   <sheetData>
     <row r="3" spans="1:9" ht="16" thickBot="1"/>
     <row r="4" spans="1:9" ht="16" thickBot="1">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:9" ht="16" thickBot="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
+        <v>654</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="34" t="s">
         <v>655</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="33" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="22" t="s">
         <v>656</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="22" t="s">
+      <c r="F5" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" thickBot="1">
+      <c r="A6" s="36" t="s">
+        <v>659</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="34" t="s">
+        <v>658</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="22" t="s">
         <v>657</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="G6" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>617</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16" thickBot="1">
-      <c r="A6" s="35" t="s">
-        <v>660</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="22" t="s">
-        <v>658</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>618</v>
-      </c>
       <c r="I6" s="24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1">
-      <c r="A7" s="35">
+      <c r="A7" s="36">
         <v>16</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33">
+      <c r="B7" s="35"/>
+      <c r="C7" s="34">
         <v>16</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="22">
         <v>8</v>
       </c>
@@ -4595,7 +4593,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -4621,7 +4619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -4633,13 +4631,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="25" t="s">
@@ -5113,16 +5111,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5130,7 +5128,7 @@
         <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>173</v>
@@ -5139,7 +5137,7 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -8363,16 +8361,16 @@
         <v>541</v>
       </c>
       <c r="B221" t="s">
+        <v>652</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>653</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -8482,7 +8480,7 @@
         <v>568</v>
       </c>
       <c r="B228" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>172</v>
@@ -8491,7 +8489,7 @@
         <v>321</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -8516,16 +8514,16 @@
         <v>570</v>
       </c>
       <c r="B230" t="s">
+        <v>631</v>
+      </c>
+      <c r="C230" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="D230" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -8550,7 +8548,7 @@
         <v>572</v>
       </c>
       <c r="B232" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>172</v>
@@ -8559,7 +8557,7 @@
         <v>321</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -8754,7 +8752,7 @@
         <v>584</v>
       </c>
       <c r="B244" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>552</v>
@@ -8763,7 +8761,7 @@
         <v>321</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -8771,16 +8769,16 @@
         <v>585</v>
       </c>
       <c r="B245" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -8788,7 +8786,7 @@
         <v>586</v>
       </c>
       <c r="B246" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>552</v>
@@ -8797,7 +8795,7 @@
         <v>321</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -8805,16 +8803,16 @@
         <v>587</v>
       </c>
       <c r="B247" t="s">
+        <v>637</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>639</v>
-      </c>
       <c r="D247" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -8907,7 +8905,7 @@
         <v>593</v>
       </c>
       <c r="B253" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>172</v>
@@ -8916,7 +8914,7 @@
         <v>321</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -8958,7 +8956,7 @@
         <v>596</v>
       </c>
       <c r="B256" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>172</v>
@@ -8967,7 +8965,7 @@
         <v>321</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -8992,16 +8990,16 @@
         <v>598</v>
       </c>
       <c r="B258" t="s">
+        <v>647</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating register macros and readme file for register layouts
</commit_message>
<xml_diff>
--- a/sim/goblin-core_opcodes.xlsx
+++ b/sim/goblin-core_opcodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="667">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -1730,9 +1730,6 @@
     <t>Greater-Than</t>
   </si>
   <si>
-    <t>Grater-Than+EQ</t>
-  </si>
-  <si>
     <t>Less-Than</t>
   </si>
   <si>
@@ -2308,6 +2305,12 @@
   </si>
   <si>
     <t>Ra.Rb,Rt</t>
+  </si>
+  <si>
+    <t>Mnemonic</t>
+  </si>
+  <si>
+    <t>Greater-Than+EQ</t>
   </si>
 </sst>
 </file>
@@ -2623,8 +2626,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2897,7 +2904,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2989,6 +2996,8 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3080,6 +3089,8 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3411,8 +3422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3457,7 +3468,7 @@
         <v>347</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>11</v>
+        <v>665</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>25</v>
@@ -3664,16 +3675,16 @@
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>650</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>651</v>
       </c>
       <c r="C11" s="22">
         <v>16</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -4071,10 +4082,10 @@
         <v>64</v>
       </c>
       <c r="G39" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>548</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>549</v>
       </c>
       <c r="I39" s="19" t="s">
         <v>156</v>
@@ -4085,10 +4096,10 @@
         <v>65</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>156</v>
@@ -4099,10 +4110,10 @@
         <v>66</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I41" s="19" t="s">
         <v>156</v>
@@ -4113,10 +4124,10 @@
         <v>67</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I42" s="19" t="s">
         <v>156</v>
@@ -4124,16 +4135,16 @@
     </row>
     <row r="43" spans="4:12">
       <c r="D43" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I43" s="19" t="s">
         <v>156</v>
@@ -4141,16 +4152,16 @@
     </row>
     <row r="44" spans="4:12">
       <c r="D44" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G44" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>601</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>602</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>156</v>
@@ -4161,10 +4172,10 @@
         <v>70</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>156</v>
@@ -4175,10 +4186,10 @@
         <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>156</v>
@@ -4186,22 +4197,22 @@
     </row>
     <row r="47" spans="4:12">
       <c r="D47" s="33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>606</v>
+        <v>624</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>608</v>
+        <v>625</v>
       </c>
       <c r="I47" s="19" t="s">
         <v>156</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="48" spans="4:12">
@@ -4210,10 +4221,10 @@
         <v>73</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>625</v>
+        <v>598</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
       <c r="I48" s="19" t="s">
         <v>156</v>
@@ -4225,10 +4236,10 @@
         <v>74</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>599</v>
+        <v>610</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="I49" s="19" t="s">
         <v>156</v>
@@ -4240,10 +4251,10 @@
         <v>75</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>156</v>
@@ -4255,10 +4266,10 @@
         <v>76</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>614</v>
+        <v>156</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>615</v>
+        <v>156</v>
       </c>
       <c r="I51" s="19" t="s">
         <v>156</v>
@@ -4415,7 +4426,7 @@
         <v>482</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>488</v>
+        <v>666</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>321</v>
@@ -4429,7 +4440,7 @@
         <v>483</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I63" s="19" t="s">
         <v>321</v>
@@ -4443,7 +4454,7 @@
         <v>484</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I64" s="19" t="s">
         <v>321</v>
@@ -4457,7 +4468,7 @@
         <v>485</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I65" s="19" t="s">
         <v>321</v>
@@ -4468,10 +4479,10 @@
         <v>91</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>321</v>
@@ -4523,52 +4534,52 @@
     </row>
     <row r="5" spans="1:9" ht="16" thickBot="1">
       <c r="A5" s="36" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="34" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" thickBot="1">
       <c r="A6" s="36" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="34" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="22" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1">
@@ -4593,7 +4604,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -5111,16 +5122,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5128,7 +5139,7 @@
         <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>173</v>
@@ -5137,7 +5148,7 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5196,16 +5207,16 @@
         <v>54</v>
       </c>
       <c r="B34" t="s">
+        <v>491</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6831,7 +6842,7 @@
         <v>348</v>
       </c>
       <c r="B131" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>189</v>
@@ -6840,7 +6851,7 @@
         <v>321</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -6848,7 +6859,7 @@
         <v>349</v>
       </c>
       <c r="B132" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>189</v>
@@ -6857,7 +6868,7 @@
         <v>321</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -6865,7 +6876,7 @@
         <v>350</v>
       </c>
       <c r="B133" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>189</v>
@@ -6874,7 +6885,7 @@
         <v>321</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -6882,7 +6893,7 @@
         <v>351</v>
       </c>
       <c r="B134" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>189</v>
@@ -6891,7 +6902,7 @@
         <v>321</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -7103,7 +7114,7 @@
         <v>364</v>
       </c>
       <c r="B147" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>189</v>
@@ -7112,7 +7123,7 @@
         <v>321</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -7120,7 +7131,7 @@
         <v>365</v>
       </c>
       <c r="B148" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>189</v>
@@ -7129,7 +7140,7 @@
         <v>321</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -7137,7 +7148,7 @@
         <v>366</v>
       </c>
       <c r="B149" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>189</v>
@@ -7146,7 +7157,7 @@
         <v>321</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -7154,7 +7165,7 @@
         <v>367</v>
       </c>
       <c r="B150" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>189</v>
@@ -7163,7 +7174,7 @@
         <v>321</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -7375,16 +7386,16 @@
         <v>380</v>
       </c>
       <c r="B163" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -7392,16 +7403,16 @@
         <v>381</v>
       </c>
       <c r="B164" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -7409,16 +7420,16 @@
         <v>382</v>
       </c>
       <c r="B165" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -7426,16 +7437,16 @@
         <v>383</v>
       </c>
       <c r="B166" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -7443,16 +7454,16 @@
         <v>384</v>
       </c>
       <c r="B167" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -7460,16 +7471,16 @@
         <v>385</v>
       </c>
       <c r="B168" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -7647,7 +7658,7 @@
         <v>396</v>
       </c>
       <c r="B179" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>156</v>
@@ -7656,7 +7667,7 @@
         <v>156</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -7664,16 +7675,16 @@
         <v>397</v>
       </c>
       <c r="B180" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -7817,16 +7828,16 @@
         <v>406</v>
       </c>
       <c r="B189" t="s">
+        <v>552</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="D189" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E189" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -7834,16 +7845,16 @@
         <v>407</v>
       </c>
       <c r="B190" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -7919,16 +7930,16 @@
         <v>412</v>
       </c>
       <c r="B195" t="s">
+        <v>556</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E195" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -7936,16 +7947,16 @@
         <v>413</v>
       </c>
       <c r="B196" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -8089,16 +8100,16 @@
         <v>422</v>
       </c>
       <c r="B205" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -8106,16 +8117,16 @@
         <v>423</v>
       </c>
       <c r="B206" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -8191,38 +8202,38 @@
         <v>428</v>
       </c>
       <c r="B211" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B212" t="s">
+        <v>563</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C212" s="1" t="s">
-        <v>565</v>
-      </c>
       <c r="D212" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B213" t="s">
         <v>156</v>
@@ -8239,7 +8250,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B214" t="s">
         <v>156</v>
@@ -8256,7 +8267,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B215" t="s">
         <v>156</v>
@@ -8273,7 +8284,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B216" t="s">
         <v>156</v>
@@ -8290,7 +8301,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B217" t="s">
         <v>156</v>
@@ -8307,7 +8318,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B218" t="s">
         <v>156</v>
@@ -8324,7 +8335,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B219" t="s">
         <v>156</v>
@@ -8341,7 +8352,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B220" t="s">
         <v>156</v>
@@ -8358,24 +8369,24 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B221" t="s">
+        <v>651</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B222" t="s">
         <v>156</v>
@@ -8392,7 +8403,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B223" t="s">
         <v>156</v>
@@ -8409,7 +8420,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B224" t="s">
         <v>156</v>
@@ -8426,7 +8437,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B225" t="s">
         <v>156</v>
@@ -8443,7 +8454,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B226" t="s">
         <v>156</v>
@@ -8460,7 +8471,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B227" t="s">
         <v>304</v>
@@ -8477,10 +8488,10 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B228" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>172</v>
@@ -8489,12 +8500,12 @@
         <v>321</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B229" t="s">
         <v>156</v>
@@ -8511,24 +8522,24 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B230" t="s">
+        <v>630</v>
+      </c>
+      <c r="C230" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="D230" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>632</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B231" t="s">
         <v>156</v>
@@ -8545,10 +8556,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B232" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>172</v>
@@ -8557,12 +8568,12 @@
         <v>321</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B233" t="s">
         <v>156</v>
@@ -8579,7 +8590,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B234" t="s">
         <v>156</v>
@@ -8596,7 +8607,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B235" t="s">
         <v>156</v>
@@ -8613,7 +8624,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B236" t="s">
         <v>156</v>
@@ -8630,7 +8641,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B237" t="s">
         <v>305</v>
@@ -8647,7 +8658,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B238" t="s">
         <v>306</v>
@@ -8664,7 +8675,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B239" t="s">
         <v>307</v>
@@ -8681,7 +8692,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B240" t="s">
         <v>156</v>
@@ -8698,7 +8709,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B241" t="s">
         <v>156</v>
@@ -8715,7 +8726,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B242" t="s">
         <v>156</v>
@@ -8732,7 +8743,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B243" t="s">
         <v>156</v>
@@ -8749,75 +8760,75 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B244" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B245" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B246" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B247" t="s">
+        <v>636</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>638</v>
-      </c>
       <c r="D247" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B248" t="s">
         <v>156</v>
@@ -8834,7 +8845,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B249" t="s">
         <v>156</v>
@@ -8851,7 +8862,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B250" t="s">
         <v>156</v>
@@ -8868,7 +8879,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B251" t="s">
         <v>156</v>
@@ -8885,7 +8896,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B252" t="s">
         <v>156</v>
@@ -8902,10 +8913,10 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B253" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>172</v>
@@ -8914,12 +8925,12 @@
         <v>321</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B254" t="s">
         <v>156</v>
@@ -8936,7 +8947,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B255" t="s">
         <v>156</v>
@@ -8953,10 +8964,10 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B256" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>172</v>
@@ -8965,12 +8976,12 @@
         <v>321</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B257" t="s">
         <v>156</v>
@@ -8987,19 +8998,19 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B258" t="s">
+        <v>646</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first clean compile; fleshed out the makefiles; fixed issues with macros
</commit_message>
<xml_diff>
--- a/sim/goblin-core_opcodes.xlsx
+++ b/sim/goblin-core_opcodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23580" windowHeight="13360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19960" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="669">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2311,6 +2311,12 @@
   </si>
   <si>
     <t>Greater-Than+EQ</t>
+  </si>
+  <si>
+    <t>AMO.CAS.SQ</t>
+  </si>
+  <si>
+    <t>AMO: Compare and Swap</t>
   </si>
 </sst>
 </file>
@@ -2626,8 +2632,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2904,7 +2922,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2998,6 +3016,12 @@
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3091,6 +3115,12 @@
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3423,7 +3453,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4514,7 +4544,7 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4630,8 +4660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128:E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4679,7 +4709,7 @@
         <v>156</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>157</v>
@@ -6553,16 +6583,16 @@
         <v>139</v>
       </c>
       <c r="B114" t="s">
-        <v>156</v>
+        <v>667</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>156</v>
+        <v>668</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -6740,16 +6770,16 @@
         <v>150</v>
       </c>
       <c r="B125" t="s">
-        <v>304</v>
+        <v>156</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>308</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -6757,16 +6787,16 @@
         <v>151</v>
       </c>
       <c r="B126" t="s">
-        <v>305</v>
+        <v>156</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>309</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -6774,16 +6804,16 @@
         <v>152</v>
       </c>
       <c r="B127" t="s">
-        <v>306</v>
+        <v>156</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>310</v>
+        <v>156</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -6791,16 +6821,16 @@
         <v>153</v>
       </c>
       <c r="B128" t="s">
-        <v>307</v>
+        <v>156</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>311</v>
+        <v>156</v>
       </c>
     </row>
     <row r="129" spans="1:5">

</xml_diff>

<commit_message>
checking in documentation and a few nice debug messages
</commit_message>
<xml_diff>
--- a/sim/goblin-core_opcodes.xlsx
+++ b/sim/goblin-core_opcodes.xlsx
@@ -3453,7 +3453,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3468,7 +3468,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>665</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
@@ -4660,8 +4660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128:E128"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>